<commit_message>
copy PCT_DA_POP values from 2024 to 2025 inputs for both Munis and CCAs
also ensured all records sorted A to Z by community name
</commit_message>
<xml_diff>
--- a/input/community_cohort_inputs_2024.xlsx
+++ b/input/community_cohort_inputs_2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amcadams\GitHub\community-cohort-tool\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228A909B-0741-40CF-96A4-37B18A286042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D042E3-1ECF-4E95-B6BF-143D8BAF301D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23055" yWindow="7095" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19425" yWindow="-14550" windowWidth="19815" windowHeight="13860" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FACTORS_MUNI" sheetId="1" r:id="rId1"/>
@@ -2900,7 +2900,7 @@
   <dimension ref="A1:L285"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15169,6 +15169,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L285" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L285">
+      <sortCondition ref="B1:B285"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -15179,8 +15184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15253,7 +15258,7 @@
         <v>29781.962918929472</v>
       </c>
       <c r="H2" s="8">
-        <f t="shared" ref="H2:H33" si="0">LN(G2)</f>
+        <f>LN(G2)</f>
         <v>10.301658218066086</v>
       </c>
       <c r="I2" s="8">
@@ -15261,7 +15266,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J2" s="8">
-        <f t="shared" ref="J2:J33" si="1">LN(C2)</f>
+        <f>LN(C2)</f>
         <v>11.271334499718714</v>
       </c>
     </row>
@@ -15289,7 +15294,7 @@
         <v>29183.470760991047</v>
       </c>
       <c r="H3" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G3)</f>
         <v>10.281357758149285</v>
       </c>
       <c r="I3" s="8">
@@ -15297,7 +15302,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J3" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C3)</f>
         <v>10.959540226785442</v>
       </c>
     </row>
@@ -15325,7 +15330,7 @@
         <v>36630.808537357385</v>
       </c>
       <c r="H4" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G4)</f>
         <v>10.508644928621182</v>
       </c>
       <c r="I4" s="8">
@@ -15333,7 +15338,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J4" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C4)</f>
         <v>10.719876156208088</v>
       </c>
     </row>
@@ -15361,7 +15366,7 @@
         <v>26759.409089345005</v>
       </c>
       <c r="H5" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G5)</f>
         <v>10.194641432135315</v>
       </c>
       <c r="I5" s="8">
@@ -15369,7 +15374,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J5" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C5)</f>
         <v>11.265232461066633</v>
       </c>
     </row>
@@ -15397,7 +15402,7 @@
         <v>22214.831291047369</v>
       </c>
       <c r="H6" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G6)</f>
         <v>10.008515420970133</v>
       </c>
       <c r="I6" s="8">
@@ -15405,7 +15410,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J6" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C6)</f>
         <v>10.621327345686446</v>
       </c>
     </row>
@@ -15433,7 +15438,7 @@
         <v>23859.775398112979</v>
       </c>
       <c r="H7" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G7)</f>
         <v>10.079949282284591</v>
       </c>
       <c r="I7" s="8">
@@ -15441,7 +15446,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J7" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C7)</f>
         <v>10.598776656091799</v>
       </c>
     </row>
@@ -15469,7 +15474,7 @@
         <v>26133.449873254835</v>
       </c>
       <c r="H8" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G8)</f>
         <v>10.170971377096217</v>
       </c>
       <c r="I8" s="8">
@@ -15477,7 +15482,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J8" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C8)</f>
         <v>10.899305052792558</v>
       </c>
     </row>
@@ -15505,7 +15510,7 @@
         <v>36735.192125354428</v>
       </c>
       <c r="H9" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G9)</f>
         <v>10.511490488076211</v>
       </c>
       <c r="I9" s="8">
@@ -15513,7 +15518,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J9" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C9)</f>
         <v>11.424568504489276</v>
       </c>
     </row>
@@ -15541,7 +15546,7 @@
         <v>25219.502230169608</v>
       </c>
       <c r="H10" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G10)</f>
         <v>10.135372872217454</v>
       </c>
       <c r="I10" s="8">
@@ -15549,7 +15554,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J10" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C10)</f>
         <v>11.042541573338868</v>
       </c>
     </row>
@@ -15577,7 +15582,7 @@
         <v>37894.449282783746</v>
       </c>
       <c r="H11" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G11)</f>
         <v>10.542559923426021</v>
       </c>
       <c r="I11" s="8">
@@ -15585,7 +15590,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J11" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C11)</f>
         <v>11.784247621980015</v>
       </c>
     </row>
@@ -15613,7 +15618,7 @@
         <v>36075.195438752475</v>
       </c>
       <c r="H12" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G12)</f>
         <v>10.493360801195033</v>
       </c>
       <c r="I12" s="8">
@@ -15621,7 +15626,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J12" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C12)</f>
         <v>11.186628731268636</v>
       </c>
     </row>
@@ -15649,7 +15654,7 @@
         <v>22715.91864694142</v>
       </c>
       <c r="H13" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G13)</f>
         <v>10.030821219680002</v>
       </c>
       <c r="I13" s="8">
@@ -15657,7 +15662,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J13" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C13)</f>
         <v>10.861775678346413</v>
       </c>
     </row>
@@ -15685,7 +15690,7 @@
         <v>28591.184047535768</v>
       </c>
       <c r="H14" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G14)</f>
         <v>10.26085369920296</v>
       </c>
       <c r="I14" s="8">
@@ -15693,7 +15698,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J14" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C14)</f>
         <v>10.751724821165267</v>
       </c>
     </row>
@@ -15721,7 +15726,7 @@
         <v>28005.18938199283</v>
       </c>
       <c r="H15" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G15)</f>
         <v>10.24014510705609</v>
       </c>
       <c r="I15" s="8">
@@ -15729,7 +15734,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J15" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C15)</f>
         <v>11.133647719106873</v>
       </c>
     </row>
@@ -15757,7 +15762,7 @@
         <v>24076.707312769591</v>
       </c>
       <c r="H16" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G16)</f>
         <v>10.089000150570135</v>
       </c>
       <c r="I16" s="8">
@@ -15765,7 +15770,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J16" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C16)</f>
         <v>10.58021186207427</v>
       </c>
     </row>
@@ -15793,7 +15798,7 @@
         <v>21469.650112295898</v>
       </c>
       <c r="H17" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G17)</f>
         <v>9.9743955941539113</v>
       </c>
       <c r="I17" s="8">
@@ -15801,7 +15806,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J17" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C17)</f>
         <v>10.675757618537041</v>
       </c>
     </row>
@@ -15829,7 +15834,7 @@
         <v>28893.901446860826</v>
       </c>
       <c r="H18" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G18)</f>
         <v>10.27138582923215</v>
       </c>
       <c r="I18" s="8">
@@ -15837,7 +15842,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J18" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C18)</f>
         <v>11.208816407253209</v>
       </c>
     </row>
@@ -15865,7 +15870,7 @@
         <v>28425.701498510003</v>
       </c>
       <c r="H19" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G19)</f>
         <v>10.25504899724157</v>
       </c>
       <c r="I19" s="8">
@@ -15873,7 +15878,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J19" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C19)</f>
         <v>10.681154582882046</v>
       </c>
     </row>
@@ -15901,7 +15906,7 @@
         <v>35225.061560690148</v>
       </c>
       <c r="H20" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G20)</f>
         <v>10.469513084407374</v>
       </c>
       <c r="I20" s="8">
@@ -15909,7 +15914,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J20" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C20)</f>
         <v>11.34499233708158</v>
       </c>
     </row>
@@ -15937,7 +15942,7 @@
         <v>23769.104741285177</v>
       </c>
       <c r="H21" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G21)</f>
         <v>10.076141896257711</v>
       </c>
       <c r="I21" s="8">
@@ -15945,7 +15950,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J21" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C21)</f>
         <v>10.366038545019112</v>
       </c>
     </row>
@@ -15973,7 +15978,7 @@
         <v>20068.64706722321</v>
       </c>
       <c r="H22" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G22)</f>
         <v>9.9069140288167965</v>
       </c>
       <c r="I22" s="8">
@@ -15981,7 +15986,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J22" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C22)</f>
         <v>11.033236645950517</v>
       </c>
     </row>
@@ -16009,7 +16014,7 @@
         <v>35798.347341622932</v>
       </c>
       <c r="H23" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G23)</f>
         <v>10.4856570076814</v>
       </c>
       <c r="I23" s="8">
@@ -16017,7 +16022,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J23" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C23)</f>
         <v>11.124253569929543</v>
       </c>
     </row>
@@ -16045,7 +16050,7 @@
         <v>46846.950603594269</v>
       </c>
       <c r="H24" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G24)</f>
         <v>10.754641197044362</v>
       </c>
       <c r="I24" s="8">
@@ -16053,7 +16058,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J24" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C24)</f>
         <v>11.695443543333054</v>
       </c>
     </row>
@@ -16081,7 +16086,7 @@
         <v>19496.747283112865</v>
       </c>
       <c r="H25" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G25)</f>
         <v>9.8780029246439582</v>
       </c>
       <c r="I25" s="8">
@@ -16089,7 +16094,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J25" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C25)</f>
         <v>10.23249671840507</v>
       </c>
     </row>
@@ -16117,7 +16122,7 @@
         <v>50238.080062177505</v>
       </c>
       <c r="H26" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G26)</f>
         <v>10.824528585088956</v>
       </c>
       <c r="I26" s="8">
@@ -16125,7 +16130,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J26" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C26)</f>
         <v>11.842557927322733</v>
       </c>
     </row>
@@ -16153,7 +16158,7 @@
         <v>24183.227088594656</v>
       </c>
       <c r="H27" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G27)</f>
         <v>10.093414576330424</v>
       </c>
       <c r="I27" s="8">
@@ -16161,7 +16166,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J27" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C27)</f>
         <v>9.6394365405359217</v>
       </c>
     </row>
@@ -16189,7 +16194,7 @@
         <v>21417.158705556936</v>
       </c>
       <c r="H28" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G28)</f>
         <v>9.9719476884039793</v>
       </c>
       <c r="I28" s="8">
@@ -16197,7 +16202,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J28" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C28)</f>
         <v>10.822013139346193</v>
       </c>
     </row>
@@ -16225,7 +16230,7 @@
         <v>31104.216173608947</v>
       </c>
       <c r="H29" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G29)</f>
         <v>10.345098657262023</v>
       </c>
       <c r="I29" s="8">
@@ -16233,7 +16238,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J29" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C29)</f>
         <v>11.411708267576127</v>
       </c>
     </row>
@@ -16261,7 +16266,7 @@
         <v>26489.692790960624</v>
       </c>
       <c r="H30" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G30)</f>
         <v>10.184510985028638</v>
       </c>
       <c r="I30" s="8">
@@ -16269,7 +16274,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J30" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C30)</f>
         <v>10.670062201650889</v>
       </c>
     </row>
@@ -16297,7 +16302,7 @@
         <v>22188.154718559199</v>
       </c>
       <c r="H31" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G31)</f>
         <v>10.007313854224511</v>
       </c>
       <c r="I31" s="8">
@@ -16305,7 +16310,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J31" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C31)</f>
         <v>10.594327926998156</v>
       </c>
     </row>
@@ -16333,7 +16338,7 @@
         <v>26852.74541380454</v>
       </c>
       <c r="H32" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G32)</f>
         <v>10.198123344758416</v>
       </c>
       <c r="I32" s="8">
@@ -16341,7 +16346,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J32" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C32)</f>
         <v>10.979299540216626</v>
       </c>
     </row>
@@ -16369,7 +16374,7 @@
         <v>25593.444046410092</v>
       </c>
       <c r="H33" s="8">
-        <f t="shared" si="0"/>
+        <f>LN(G33)</f>
         <v>10.150091505733409</v>
       </c>
       <c r="I33" s="8">
@@ -16377,7 +16382,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J33" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C33)</f>
         <v>11.098514046113948</v>
       </c>
     </row>
@@ -16405,7 +16410,7 @@
         <v>25495.656998544615</v>
       </c>
       <c r="H34" s="8">
-        <f t="shared" ref="H34:H65" si="2">LN(G34)</f>
+        <f>LN(G34)</f>
         <v>10.146263402858914</v>
       </c>
       <c r="I34" s="8">
@@ -16413,7 +16418,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J34" s="8">
-        <f t="shared" ref="J34:J65" si="3">LN(C34)</f>
+        <f>LN(C34)</f>
         <v>10.841627945143156</v>
       </c>
     </row>
@@ -16441,7 +16446,7 @@
         <v>39929.153202477828</v>
       </c>
       <c r="H35" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G35)</f>
         <v>10.594861992782002</v>
       </c>
       <c r="I35" s="8">
@@ -16449,7 +16454,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J35" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C35)</f>
         <v>11.018699198148646</v>
       </c>
     </row>
@@ -16477,7 +16482,7 @@
         <v>36420.264743786283</v>
       </c>
       <c r="H36" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G36)</f>
         <v>10.502880622442062</v>
       </c>
       <c r="I36" s="8">
@@ -16485,7 +16490,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J36" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C36)</f>
         <v>11.371926832804741</v>
       </c>
     </row>
@@ -16513,7 +16518,7 @@
         <v>35836.332789086635</v>
       </c>
       <c r="H37" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G37)</f>
         <v>10.486717540120567</v>
       </c>
       <c r="I37" s="8">
@@ -16521,7 +16526,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J37" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C37)</f>
         <v>11.415758724112797</v>
       </c>
     </row>
@@ -16549,7 +16554,7 @@
         <v>34816.365618341588</v>
       </c>
       <c r="H38" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G38)</f>
         <v>10.457842831606408</v>
       </c>
       <c r="I38" s="8">
@@ -16557,7 +16562,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J38" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C38)</f>
         <v>10.969093544736067</v>
       </c>
     </row>
@@ -16585,7 +16590,7 @@
         <v>56822.087243243906</v>
       </c>
       <c r="H39" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G39)</f>
         <v>10.947680389039085</v>
       </c>
       <c r="I39" s="8">
@@ -16593,7 +16598,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J39" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C39)</f>
         <v>11.519152514143558</v>
       </c>
     </row>
@@ -16621,7 +16626,7 @@
         <v>79566.128920131596</v>
       </c>
       <c r="H40" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G40)</f>
         <v>11.284343765196068</v>
       </c>
       <c r="I40" s="8">
@@ -16629,7 +16634,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J40" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C40)</f>
         <v>11.807663750113845</v>
       </c>
     </row>
@@ -16657,7 +16662,7 @@
         <v>41107.127198575428</v>
       </c>
       <c r="H41" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G41)</f>
         <v>10.623936796607902</v>
       </c>
       <c r="I41" s="8">
@@ -16665,7 +16670,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J41" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C41)</f>
         <v>11.413866423563936</v>
       </c>
     </row>
@@ -16693,7 +16698,7 @@
         <v>45272.22336589529</v>
       </c>
       <c r="H42" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G42)</f>
         <v>10.720448952674284</v>
       </c>
       <c r="I42" s="8">
@@ -16701,7 +16706,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J42" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C42)</f>
         <v>11.490262864324347</v>
       </c>
     </row>
@@ -16729,7 +16734,7 @@
         <v>34937.524265830849</v>
       </c>
       <c r="H43" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G43)</f>
         <v>10.461316724446935</v>
       </c>
       <c r="I43" s="8">
@@ -16737,7 +16742,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J43" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C43)</f>
         <v>11.153539002752964</v>
       </c>
     </row>
@@ -16765,7 +16770,7 @@
         <v>30994.727023960724</v>
       </c>
       <c r="H44" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G44)</f>
         <v>10.341572372998051</v>
       </c>
       <c r="I44" s="8">
@@ -16773,7 +16778,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J44" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C44)</f>
         <v>11.162100201356512</v>
       </c>
     </row>
@@ -16801,7 +16806,7 @@
         <v>28558.967006281608</v>
       </c>
       <c r="H45" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G45)</f>
         <v>10.259726246551555</v>
       </c>
       <c r="I45" s="8">
@@ -16809,7 +16814,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J45" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C45)</f>
         <v>11.142419041883034</v>
       </c>
     </row>
@@ -16837,7 +16842,7 @@
         <v>29392.546054372368</v>
       </c>
       <c r="H46" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G46)</f>
         <v>10.288496385615632</v>
       </c>
       <c r="I46" s="8">
@@ -16845,7 +16850,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J46" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C46)</f>
         <v>11.180002812268926</v>
       </c>
     </row>
@@ -16873,7 +16878,7 @@
         <v>32130.420204227077</v>
       </c>
       <c r="H47" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G47)</f>
         <v>10.377558530276083</v>
       </c>
       <c r="I47" s="8">
@@ -16881,7 +16886,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J47" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C47)</f>
         <v>11.638039210746214</v>
       </c>
     </row>
@@ -16909,7 +16914,7 @@
         <v>300588.37309242727</v>
       </c>
       <c r="H48" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G48)</f>
         <v>12.613497076552385</v>
       </c>
       <c r="I48" s="8">
@@ -16917,7 +16922,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J48" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C48)</f>
         <v>11.708176264754101</v>
       </c>
     </row>
@@ -16945,7 +16950,7 @@
         <v>72965.182927549846</v>
       </c>
       <c r="H49" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G49)</f>
         <v>11.197737660157566</v>
       </c>
       <c r="I49" s="8">
@@ -16953,7 +16958,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J49" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C49)</f>
         <v>11.732529637036537</v>
       </c>
     </row>
@@ -16981,7 +16986,7 @@
         <v>89190.500021186512</v>
       </c>
       <c r="H50" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G50)</f>
         <v>11.398529810891723</v>
       </c>
       <c r="I50" s="8">
@@ -16989,7 +16994,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J50" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C50)</f>
         <v>11.58016267475325</v>
       </c>
     </row>
@@ -17017,7 +17022,7 @@
         <v>22808.426731448846</v>
       </c>
       <c r="H51" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G51)</f>
         <v>10.034885340144283</v>
       </c>
       <c r="I51" s="8">
@@ -17025,7 +17030,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J51" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C51)</f>
         <v>10.620335965381761</v>
       </c>
     </row>
@@ -17053,7 +17058,7 @@
         <v>59055.859830313871</v>
       </c>
       <c r="H52" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G52)</f>
         <v>10.986239051762389</v>
       </c>
       <c r="I52" s="8">
@@ -17061,7 +17066,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J52" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C52)</f>
         <v>11.908914510372936</v>
       </c>
     </row>
@@ -17089,7 +17094,7 @@
         <v>22529.030770653291</v>
       </c>
       <c r="H53" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G53)</f>
         <v>10.022560013000405</v>
       </c>
       <c r="I53" s="8">
@@ -17097,7 +17102,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J53" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C53)</f>
         <v>10.414346027273687</v>
       </c>
     </row>
@@ -17125,7 +17130,7 @@
         <v>35675.586686472605</v>
       </c>
       <c r="H54" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G54)</f>
         <v>10.48222188752089</v>
       </c>
       <c r="I54" s="8">
@@ -17133,7 +17138,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J54" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C54)</f>
         <v>11.220549196407191</v>
       </c>
     </row>
@@ -17161,7 +17166,7 @@
         <v>39646.399143461444</v>
       </c>
       <c r="H55" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G55)</f>
         <v>10.58775540688503</v>
       </c>
       <c r="I55" s="8">
@@ -17169,7 +17174,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J55" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C55)</f>
         <v>11.581720451532894</v>
       </c>
     </row>
@@ -17197,7 +17202,7 @@
         <v>26672.301145177298</v>
       </c>
       <c r="H56" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G56)</f>
         <v>10.191380895612847</v>
       </c>
       <c r="I56" s="8">
@@ -17205,7 +17210,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J56" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C56)</f>
         <v>10.228948319331135</v>
       </c>
     </row>
@@ -17233,7 +17238,7 @@
         <v>40035.098278045916</v>
       </c>
       <c r="H57" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G57)</f>
         <v>10.597511805306917</v>
       </c>
       <c r="I57" s="8">
@@ -17241,7 +17246,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J57" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C57)</f>
         <v>11.15551198746229</v>
       </c>
     </row>
@@ -17269,7 +17274,7 @@
         <v>32488.229724070618</v>
       </c>
       <c r="H58" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G58)</f>
         <v>10.388633140384924</v>
       </c>
       <c r="I58" s="8">
@@ -17277,7 +17282,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J58" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C58)</f>
         <v>11.355960565133584</v>
       </c>
     </row>
@@ -17305,7 +17310,7 @@
         <v>28270.630949512713</v>
       </c>
       <c r="H59" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G59)</f>
         <v>10.249578769133757</v>
       </c>
       <c r="I59" s="8">
@@ -17313,7 +17318,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J59" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C59)</f>
         <v>10.910628437707077</v>
       </c>
     </row>
@@ -17341,7 +17346,7 @@
         <v>15975.675396810533</v>
       </c>
       <c r="H60" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G60)</f>
         <v>9.6788225567126283</v>
       </c>
       <c r="I60" s="8">
@@ -17349,7 +17354,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J60" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C60)</f>
         <v>9.9584033101322422</v>
       </c>
     </row>
@@ -17377,7 +17382,7 @@
         <v>28989.071852351441</v>
       </c>
       <c r="H61" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G61)</f>
         <v>10.274674205271799</v>
       </c>
       <c r="I61" s="8">
@@ -17385,7 +17390,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J61" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C61)</f>
         <v>10.961119550511514</v>
       </c>
     </row>
@@ -17413,7 +17418,7 @@
         <v>22032.401491644319</v>
       </c>
       <c r="H62" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G62)</f>
         <v>10.000269443916245</v>
       </c>
       <c r="I62" s="8">
@@ -17421,7 +17426,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J62" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C62)</f>
         <v>10.815933974053493</v>
       </c>
     </row>
@@ -17449,7 +17454,7 @@
         <v>19890.128188207571</v>
       </c>
       <c r="H63" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G63)</f>
         <v>9.8979788166843417</v>
       </c>
       <c r="I63" s="8">
@@ -17457,7 +17462,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J63" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C63)</f>
         <v>10.690488179953238</v>
       </c>
     </row>
@@ -17485,7 +17490,7 @@
         <v>22587.157447590638</v>
       </c>
       <c r="H64" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G64)</f>
         <v>10.025136769211192</v>
       </c>
       <c r="I64" s="8">
@@ -17493,7 +17498,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J64" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C64)</f>
         <v>10.457781820152896</v>
       </c>
     </row>
@@ -17521,7 +17526,7 @@
         <v>20444.684613386424</v>
       </c>
       <c r="H65" s="8">
-        <f t="shared" si="2"/>
+        <f>LN(G65)</f>
         <v>9.925478206579804</v>
       </c>
       <c r="I65" s="8">
@@ -17529,7 +17534,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J65" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C65)</f>
         <v>10.645659832072177</v>
       </c>
     </row>
@@ -17557,7 +17562,7 @@
         <v>21576.111253465962</v>
       </c>
       <c r="H66" s="8">
-        <f t="shared" ref="H66:H97" si="4">LN(G66)</f>
+        <f>LN(G66)</f>
         <v>9.9793420211589776</v>
       </c>
       <c r="I66" s="8">
@@ -17565,7 +17570,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J66" s="8">
-        <f t="shared" ref="J66:J78" si="5">LN(C66)</f>
+        <f>LN(C66)</f>
         <v>10.587832789144938</v>
       </c>
     </row>
@@ -17593,7 +17598,7 @@
         <v>333065.25063794554</v>
       </c>
       <c r="H67" s="8">
-        <f t="shared" si="4"/>
+        <f>LN(G67)</f>
         <v>12.716093697629004</v>
       </c>
       <c r="I67" s="8">
@@ -17601,7 +17606,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J67" s="8">
-        <f t="shared" si="5"/>
+        <f>LN(C67)</f>
         <v>11.696701114251381</v>
       </c>
     </row>
@@ -17629,7 +17634,7 @@
         <v>37159.338945202151</v>
       </c>
       <c r="H68" s="8">
-        <f t="shared" si="4"/>
+        <f>LN(G68)</f>
         <v>10.52297040335087</v>
       </c>
       <c r="I68" s="8">
@@ -17637,7 +17642,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J68" s="8">
-        <f t="shared" si="5"/>
+        <f>LN(C68)</f>
         <v>11.110519326029364</v>
       </c>
     </row>
@@ -17665,7 +17670,7 @@
         <v>24033.198874881611</v>
       </c>
       <c r="H69" s="8">
-        <f t="shared" si="4"/>
+        <f>LN(G69)</f>
         <v>10.08719143992416</v>
       </c>
       <c r="I69" s="8">
@@ -17673,7 +17678,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J69" s="8">
-        <f t="shared" si="5"/>
+        <f>LN(C69)</f>
         <v>11.109411576993326</v>
       </c>
     </row>
@@ -17701,7 +17706,7 @@
         <v>21884.61384983642</v>
       </c>
       <c r="H70" s="8">
-        <f t="shared" si="4"/>
+        <f>LN(G70)</f>
         <v>9.9935391049564863</v>
       </c>
       <c r="I70" s="8">
@@ -17709,7 +17714,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J70" s="8">
-        <f t="shared" si="5"/>
+        <f>LN(C70)</f>
         <v>10.166385862410166</v>
       </c>
     </row>
@@ -17737,7 +17742,7 @@
         <v>24733.163421129382</v>
       </c>
       <c r="H71" s="8">
-        <f t="shared" si="4"/>
+        <f>LN(G71)</f>
         <v>10.115900270698107</v>
       </c>
       <c r="I71" s="8">
@@ -17745,7 +17750,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J71" s="8">
-        <f t="shared" si="5"/>
+        <f>LN(C71)</f>
         <v>11.073508093961442</v>
       </c>
     </row>
@@ -17773,7 +17778,7 @@
         <v>18823.672719654594</v>
       </c>
       <c r="H72" s="8">
-        <f t="shared" si="4"/>
+        <f>LN(G72)</f>
         <v>9.8428705439223627</v>
       </c>
       <c r="I72" s="8">
@@ -17781,7 +17786,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J72" s="8">
-        <f t="shared" si="5"/>
+        <f>LN(C72)</f>
         <v>10.283077283646394</v>
       </c>
     </row>
@@ -17809,7 +17814,7 @@
         <v>20607.040770706662</v>
       </c>
       <c r="H73" s="8">
-        <f t="shared" si="4"/>
+        <f>LN(G73)</f>
         <v>9.9333880813682498</v>
       </c>
       <c r="I73" s="8">
@@ -17817,7 +17822,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J73" s="8">
-        <f t="shared" si="5"/>
+        <f>LN(C73)</f>
         <v>10.501232637302897</v>
       </c>
     </row>
@@ -17845,7 +17850,7 @@
         <v>24656.424357756732</v>
       </c>
       <c r="H74" s="8">
-        <f t="shared" si="4"/>
+        <f>LN(G74)</f>
         <v>10.112792768547282</v>
       </c>
       <c r="I74" s="8">
@@ -17853,7 +17858,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J74" s="8">
-        <f t="shared" si="5"/>
+        <f>LN(C74)</f>
         <v>11.151188899637063</v>
       </c>
     </row>
@@ -17881,7 +17886,7 @@
         <v>21181.048170526352</v>
       </c>
       <c r="H75" s="8">
-        <f t="shared" si="4"/>
+        <f>LN(G75)</f>
         <v>9.9608621066242797</v>
       </c>
       <c r="I75" s="8">
@@ -17889,7 +17894,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J75" s="8">
-        <f t="shared" si="5"/>
+        <f>LN(C75)</f>
         <v>10.754933202877913</v>
       </c>
     </row>
@@ -17917,7 +17922,7 @@
         <v>28285.913018486506</v>
       </c>
       <c r="H76" s="8">
-        <f t="shared" si="4"/>
+        <f>LN(G76)</f>
         <v>10.250119186502767</v>
       </c>
       <c r="I76" s="8">
@@ -17925,7 +17930,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J76" s="8">
-        <f t="shared" si="5"/>
+        <f>LN(C76)</f>
         <v>11.128605801481278</v>
       </c>
     </row>
@@ -17953,7 +17958,7 @@
         <v>55141.258168912616</v>
       </c>
       <c r="H77" s="8">
-        <f t="shared" si="4"/>
+        <f>LN(G77)</f>
         <v>10.917653502034417</v>
       </c>
       <c r="I77" s="8">
@@ -17961,7 +17966,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J77" s="8">
-        <f t="shared" si="5"/>
+        <f>LN(C77)</f>
         <v>11.765368929029385</v>
       </c>
     </row>
@@ -17989,7 +17994,7 @@
         <v>23467.390959382756</v>
       </c>
       <c r="H78" s="8">
-        <f t="shared" si="4"/>
+        <f>LN(G78)</f>
         <v>10.063367117748141</v>
       </c>
       <c r="I78" s="8">
@@ -17997,11 +18002,16 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J78" s="8">
-        <f t="shared" si="5"/>
+        <f>LN(C78)</f>
         <v>10.307932326760856</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J78" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J78">
+      <sortCondition ref="B1:B78"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -18122,7 +18132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>